<commit_message>
Traditional demand of test system 1
</commit_message>
<xml_diff>
--- a/Traditional power demand of test system 1.xlsx
+++ b/Traditional power demand of test system 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neuqeducn-my.sharepoint.com/personal/qiaowenjie_neuq_edu_cn/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\GithubClone\supplementary files of collaborative operation of IES and TN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_AD4DA82427541F7ACA7EB830A00F368E6AE8DE11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FE5A983-D56D-4FE6-82BC-1A062376722E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12642B67-34F9-4823-866B-FC086423497E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-107" yWindow="-107" windowWidth="41174" windowHeight="22550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -426,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AA41" sqref="AA41"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,10 +556,10 @@
         <v>1.1539999999999999</v>
       </c>
       <c r="N2">
-        <v>4.4677179999999996</v>
+        <v>5.4677179999999996</v>
       </c>
       <c r="O2">
-        <v>4.4773870000000002</v>
+        <v>5.6678980000000001</v>
       </c>
       <c r="P2">
         <v>4.4599979999999997</v>
@@ -642,40 +642,40 @@
         <v>2.8360000000000003</v>
       </c>
       <c r="N3">
-        <v>2.5835710000000001</v>
+        <v>6.5835710000000001</v>
       </c>
       <c r="O3">
-        <v>2.6423860000000001</v>
+        <v>6.9815709999999997</v>
       </c>
       <c r="P3">
-        <v>2.644781</v>
+        <v>6.644781</v>
       </c>
       <c r="Q3">
-        <v>2.6260300000000001</v>
+        <v>3.6260300000000001</v>
       </c>
       <c r="R3">
-        <v>2.6386110000000005</v>
+        <v>4.638611</v>
       </c>
       <c r="S3">
-        <v>2.5948349999999998</v>
+        <v>4.5948349999999998</v>
       </c>
       <c r="T3">
-        <v>2.551031</v>
+        <v>4.551031</v>
       </c>
       <c r="U3">
-        <v>2.5330889999999999</v>
+        <v>6.5330890000000004</v>
       </c>
       <c r="V3">
-        <v>2.5338409999999998</v>
+        <v>7.5338409999999998</v>
       </c>
       <c r="W3">
-        <v>2.5259360000000002</v>
+        <v>6.5259359999999997</v>
       </c>
       <c r="X3">
-        <v>2.7134359999999997</v>
+        <v>5.7134359999999997</v>
       </c>
       <c r="Y3">
-        <v>2.7164040000000003</v>
+        <v>5.7164039999999998</v>
       </c>
       <c r="AA3" s="1">
         <v>1</v>
@@ -728,40 +728,40 @@
         <v>2.3670000000000004</v>
       </c>
       <c r="N4">
-        <v>1.9306860000000001</v>
+        <v>4.9306859999999997</v>
       </c>
       <c r="O4">
-        <v>1.9736879999999999</v>
+        <v>5.9298700000000002</v>
       </c>
       <c r="P4">
-        <v>1.97394</v>
+        <v>5.9739399999999998</v>
       </c>
       <c r="Q4">
-        <v>1.9624780000000002</v>
+        <v>7.9624779999999999</v>
       </c>
       <c r="R4">
-        <v>1.9695199999999999</v>
+        <v>6.9695200000000002</v>
       </c>
       <c r="S4">
-        <v>1.938709</v>
+        <v>5.9387090000000002</v>
       </c>
       <c r="T4">
-        <v>1.906121</v>
+        <v>6.9061209999999997</v>
       </c>
       <c r="U4">
-        <v>1.8890710000000002</v>
+        <v>6.8890710000000004</v>
       </c>
       <c r="V4">
-        <v>1.8887510000000001</v>
+        <v>7.8887510000000001</v>
       </c>
       <c r="W4">
-        <v>1.8981060000000001</v>
+        <v>9.8981060000000003</v>
       </c>
       <c r="X4">
-        <v>1.9981059999999999</v>
+        <v>5.9981059999999999</v>
       </c>
       <c r="Y4">
-        <v>2.0189879999999998</v>
+        <v>6.0189880000000002</v>
       </c>
       <c r="AA4" s="1">
         <v>2</v>
@@ -814,40 +814,40 @@
         <v>3.0540000000000003</v>
       </c>
       <c r="N5">
-        <v>0.2949</v>
+        <v>5.2949000000000002</v>
       </c>
       <c r="O5">
-        <v>0.29580000000000001</v>
+        <v>5.3459000000000003</v>
       </c>
       <c r="P5">
-        <v>0.29630000000000001</v>
+        <v>4.2962999999999996</v>
       </c>
       <c r="Q5">
-        <v>0.29580000000000001</v>
+        <v>5.2957999999999998</v>
       </c>
       <c r="R5">
-        <v>0.29620000000000002</v>
+        <v>5.2961999999999998</v>
       </c>
       <c r="S5">
-        <v>0.29210000000000003</v>
+        <v>5.2920999999999996</v>
       </c>
       <c r="T5">
-        <v>0.28850000000000003</v>
+        <v>6.2885</v>
       </c>
       <c r="U5">
-        <v>0.29110000000000003</v>
+        <v>6.2911000000000001</v>
       </c>
       <c r="V5">
-        <v>0.28500000000000003</v>
+        <v>7.2850000000000001</v>
       </c>
       <c r="W5">
-        <v>0.27460000000000001</v>
+        <v>5.2746000000000004</v>
       </c>
       <c r="X5">
-        <v>0.25190000000000001</v>
+        <v>6.2519</v>
       </c>
       <c r="Y5">
-        <v>0.23</v>
+        <v>8.23</v>
       </c>
       <c r="AA5" s="1">
         <v>3</v>
@@ -900,40 +900,40 @@
         <v>3.3280000000000003</v>
       </c>
       <c r="N6">
-        <v>0.40640000000000004</v>
+        <v>4.4063999999999997</v>
       </c>
       <c r="O6">
-        <v>0.43590000000000007</v>
+        <v>4.9874000000000001</v>
       </c>
       <c r="P6">
-        <v>0.44159999999999999</v>
+        <v>6.4416000000000002</v>
       </c>
       <c r="Q6">
-        <v>0.43700000000000006</v>
+        <v>7.4370000000000003</v>
       </c>
       <c r="R6">
-        <v>0.43950000000000006</v>
+        <v>5.4394999999999998</v>
       </c>
       <c r="S6">
-        <v>0.40229999999999999</v>
+        <v>6.4023000000000003</v>
       </c>
       <c r="T6">
-        <v>0.47320000000000001</v>
+        <v>6.4732000000000003</v>
       </c>
       <c r="U6">
-        <v>0.39040000000000002</v>
+        <v>5.3903999999999996</v>
       </c>
       <c r="V6">
-        <v>0.34820000000000001</v>
+        <v>6.3482000000000003</v>
       </c>
       <c r="W6">
-        <v>0.25260000000000005</v>
+        <v>5.2526000000000002</v>
       </c>
       <c r="X6">
-        <v>0.2555</v>
+        <v>6.2554999999999996</v>
       </c>
       <c r="Y6">
-        <v>0.27179999999999999</v>
+        <v>4.2717999999999998</v>
       </c>
       <c r="AA6" s="1">
         <v>4</v>
@@ -986,40 +986,40 @@
         <v>3.661</v>
       </c>
       <c r="N7">
-        <v>0.4204</v>
+        <v>7.4203999999999999</v>
       </c>
       <c r="O7">
-        <v>0.42310000000000003</v>
+        <v>7.2340400000000002</v>
       </c>
       <c r="P7">
-        <v>0.438</v>
+        <v>7.4379999999999997</v>
       </c>
       <c r="Q7">
-        <v>0.42210000000000003</v>
+        <v>6.4221000000000004</v>
       </c>
       <c r="R7">
-        <v>0.42330000000000001</v>
+        <v>4.4233000000000002</v>
       </c>
       <c r="S7">
-        <v>0.47850000000000004</v>
+        <v>6.4785000000000004</v>
       </c>
       <c r="T7">
-        <v>0.49719999999999998</v>
+        <v>5.4972000000000003</v>
       </c>
       <c r="U7">
-        <v>0.50060000000000004</v>
+        <v>6.5006000000000004</v>
       </c>
       <c r="V7">
-        <v>0.49780000000000002</v>
+        <v>5.4977999999999998</v>
       </c>
       <c r="W7">
-        <v>0.48180000000000001</v>
+        <v>4.4817999999999998</v>
       </c>
       <c r="X7">
-        <v>0.47380000000000005</v>
+        <v>4.4737999999999998</v>
       </c>
       <c r="Y7">
-        <v>0.45850000000000002</v>
+        <v>5.4584999999999999</v>
       </c>
       <c r="AA7" s="1">
         <v>5</v>
@@ -1072,40 +1072,40 @@
         <v>3.7970000000000002</v>
       </c>
       <c r="N8">
-        <v>0.32040000000000002</v>
+        <v>3.3704000000000001</v>
       </c>
       <c r="O8">
-        <v>0.32310000000000005</v>
+        <v>3.3214000000000001</v>
       </c>
       <c r="P8">
-        <v>0.33799999999999997</v>
+        <v>5.3380000000000001</v>
       </c>
       <c r="Q8">
-        <v>0.3221</v>
+        <v>4.3220999999999998</v>
       </c>
       <c r="R8">
-        <v>0.32329999999999998</v>
+        <v>7.3232999999999997</v>
       </c>
       <c r="S8">
-        <v>0.3785</v>
+        <v>4.3784999999999998</v>
       </c>
       <c r="T8">
-        <v>0.3972</v>
+        <v>4.3971999999999998</v>
       </c>
       <c r="U8">
-        <v>0.40060000000000001</v>
+        <v>4.4005999999999998</v>
       </c>
       <c r="V8">
-        <v>0.39780000000000004</v>
+        <v>4.3978000000000002</v>
       </c>
       <c r="W8">
-        <v>0.38180000000000003</v>
+        <v>4.3818000000000001</v>
       </c>
       <c r="X8">
-        <v>0.37380000000000002</v>
+        <v>4.3738000000000001</v>
       </c>
       <c r="Y8">
-        <v>0.35850000000000004</v>
+        <v>4.3585000000000003</v>
       </c>
       <c r="AA8" s="1">
         <v>6</v>
@@ -1158,40 +1158,40 @@
         <v>8.9290000000000003</v>
       </c>
       <c r="N9">
-        <v>0.79989999999999994</v>
+        <v>5.7999000000000001</v>
       </c>
       <c r="O9">
-        <v>0.81579999999999997</v>
+        <v>5.9836900000000002</v>
       </c>
       <c r="P9">
-        <v>0.80130000000000001</v>
+        <v>3.8012999999999999</v>
       </c>
       <c r="Q9">
-        <v>0.81579999999999997</v>
+        <v>5.8158000000000003</v>
       </c>
       <c r="R9">
-        <v>0.80520000000000003</v>
+        <v>5.8052000000000001</v>
       </c>
       <c r="S9">
-        <v>0.81610000000000005</v>
+        <v>5.8160999999999996</v>
       </c>
       <c r="T9">
-        <v>0.84550000000000003</v>
+        <v>6.8455000000000004</v>
       </c>
       <c r="U9">
-        <v>0.79310000000000003</v>
+        <v>5.7930999999999999</v>
       </c>
       <c r="V9">
-        <v>0.79500000000000004</v>
+        <v>3.7949999999999999</v>
       </c>
       <c r="W9">
-        <v>0.78459999999999996</v>
+        <v>3.3845999999999998</v>
       </c>
       <c r="X9">
-        <v>0.76190000000000002</v>
+        <v>5.7618999999999998</v>
       </c>
       <c r="Y9">
-        <v>0.74099999999999999</v>
+        <v>5.5410000000000004</v>
       </c>
       <c r="AA9" s="1">
         <v>7</v>
@@ -1244,40 +1244,40 @@
         <v>1.52</v>
       </c>
       <c r="N10">
-        <v>5.04E-2</v>
+        <v>6.0503999999999998</v>
       </c>
       <c r="O10">
-        <v>5.3099999999999994E-2</v>
+        <v>5.3502000000000001</v>
       </c>
       <c r="P10">
-        <v>5.7999999999999996E-2</v>
+        <v>6.3579999999999997</v>
       </c>
       <c r="Q10">
-        <v>5.21E-2</v>
+        <v>5.0521000000000003</v>
       </c>
       <c r="R10">
-        <v>5.33E-2</v>
+        <v>6.0533000000000001</v>
       </c>
       <c r="S10">
-        <v>5.8499999999999996E-2</v>
+        <v>7.0585000000000004</v>
       </c>
       <c r="T10">
-        <v>5.7200000000000001E-2</v>
+        <v>6.0571999999999999</v>
       </c>
       <c r="U10">
-        <v>5.0599999999999999E-2</v>
+        <v>4.0506000000000002</v>
       </c>
       <c r="V10">
-        <v>5.7800000000000004E-2</v>
+        <v>3.0577999999999999</v>
       </c>
       <c r="W10">
-        <v>5.1799999999999999E-2</v>
+        <v>6.0518000000000001</v>
       </c>
       <c r="X10">
-        <v>5.3800000000000001E-2</v>
+        <v>7.0537999999999998</v>
       </c>
       <c r="Y10">
-        <v>5.8499999999999996E-2</v>
+        <v>6.0585000000000004</v>
       </c>
       <c r="AA10" s="1">
         <v>8</v>

</xml_diff>